<commit_message>
Integracion parcial de reportes pdf
</commit_message>
<xml_diff>
--- a/API/dat_pl.xlsx
+++ b/API/dat_pl.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TI\Desktop\Proyectos\Fullstack\Angular -- Django\DepartmentsGestor\API\MAIN\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TI\Desktop\Proyectos\Fullstack\Angular -- Django\DepartmentsGestor\API\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,9 +23,45 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>UAPA</t>
+  </si>
+  <si>
+    <t>Id Solicitud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Departamento </t>
+  </si>
+  <si>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Departamento: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri "/>
+      </rPr>
+      <t>{{dep}}</t>
+    </r>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,16 +69,66 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Bahnschrift"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="0"/>
+      <name val="Bahnschrift"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="0"/>
+      <name val="Calibri "/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri "/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri "/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -50,12 +136,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,14 +450,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="43.5" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>